<commit_message>
Implementation of pandas in python app 	modified:   MetricsOutput.xlsx 	modified:   process_metrics_file.py
</commit_message>
<xml_diff>
--- a/MetricsOutput.xlsx
+++ b/MetricsOutput.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q72"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -702,7 +702,7 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="L17" s="1" t="inlineStr">
         <is>
           <t>FALSE</t>
         </is>
@@ -717,7 +717,7 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr">
+      <c r="O17" s="1" t="inlineStr">
         <is>
           <t>FALSE</t>
         </is>
@@ -3156,81 +3156,70 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D17:O17">
-    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="FALSE"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D28:O28">
-    <cfRule type="cellIs" priority="2" operator="lessThan" dxfId="0" stopIfTrue="0">
+    <cfRule type="cellIs" priority="1" operator="lessThan" dxfId="0" stopIfTrue="0">
       <formula>70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:O29">
-    <cfRule type="cellIs" priority="3" operator="lessThan" dxfId="0" stopIfTrue="0">
+    <cfRule type="cellIs" priority="2" operator="lessThan" dxfId="0" stopIfTrue="0">
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:O30">
-    <cfRule type="cellIs" priority="4" operator="lessThan" dxfId="0" stopIfTrue="0">
+    <cfRule type="cellIs" priority="3" operator="lessThan" dxfId="0" stopIfTrue="0">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:O34">
-    <cfRule type="cellIs" priority="5" operator="lessThan" dxfId="0" stopIfTrue="0">
+    <cfRule type="cellIs" priority="4" operator="lessThan" dxfId="0" stopIfTrue="0">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37:O37">
-    <cfRule type="cellIs" priority="6" operator="notBetween" dxfId="0" stopIfTrue="0">
-      <formula>LSL Guideline</formula>
-      <formula>USL Guideline</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D38:O38">
-    <cfRule type="cellIs" priority="7" operator="notBetween" dxfId="0" stopIfTrue="0">
+    <cfRule type="cellIs" priority="5" operator="notBetween" dxfId="0" stopIfTrue="0">
       <formula>0</formula>
       <formula>0.21</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D39:O39">
+    <cfRule type="cellIs" priority="6" operator="lessThan" dxfId="0" stopIfTrue="0">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D60:O60">
-    <cfRule type="cellIs" priority="8" operator="notBetween" dxfId="0" stopIfTrue="0">
-      <formula>0</formula>
-      <formula>0.21</formula>
+    <cfRule type="cellIs" priority="7" operator="lessThan" dxfId="0" stopIfTrue="0">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61:O61">
-    <cfRule type="cellIs" priority="9" operator="notBetween" dxfId="0" stopIfTrue="0">
-      <formula>0</formula>
-      <formula>0.21</formula>
+    <cfRule type="cellIs" priority="8" operator="lessThan" dxfId="0" stopIfTrue="0">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62:O62">
-    <cfRule type="cellIs" priority="10" operator="notBetween" dxfId="0" stopIfTrue="0">
-      <formula>0</formula>
-      <formula>0.21</formula>
+    <cfRule type="cellIs" priority="9" operator="lessThan" dxfId="0" stopIfTrue="0">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66:O66">
-    <cfRule type="cellIs" priority="11" operator="notBetween" dxfId="0" stopIfTrue="0">
-      <formula>0</formula>
-      <formula>0.21</formula>
+    <cfRule type="cellIs" priority="10" operator="lessThan" dxfId="0" stopIfTrue="0">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67:O67">
-    <cfRule type="cellIs" priority="12" operator="notBetween" dxfId="0" stopIfTrue="0">
-      <formula>0</formula>
-      <formula>0.21</formula>
+    <cfRule type="cellIs" priority="11" operator="lessThan" dxfId="0" stopIfTrue="0">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68:O68">
-    <cfRule type="cellIs" priority="13" operator="notBetween" dxfId="0" stopIfTrue="0">
-      <formula>0</formula>
-      <formula>0.21</formula>
+    <cfRule type="cellIs" priority="12" operator="lessThan" dxfId="0" stopIfTrue="0">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:O69">
-    <cfRule type="cellIs" priority="14" operator="notBetween" dxfId="0" stopIfTrue="0">
-      <formula>0</formula>
-      <formula>0.21</formula>
+    <cfRule type="cellIs" priority="13" operator="lessThan" dxfId="0" stopIfTrue="0">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>